<commit_message>
Implement total calculations and formatting in AdminAllFormatter for improved report generation. Add functionality to aggregate monthly data, calculate percentages, and format total rows. Update styles and clear excess columns in the exported Excel file.
</commit_message>
<xml_diff>
--- a/resources/views/exports/formatLaporanAkudihatinya/all.xlsx
+++ b/resources/views/exports/formatLaporanAkudihatinya/all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Program\GitHub\akudihatinya\akudihatinya-backend\resources\views\exports\formatLaporanAkudihatinya\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3F30C9-0824-417A-8664-5E51A0E79209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176005BF-5141-4531-A40E-0CB112E26210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{54DF6366-42DF-47E1-8A5D-3CF0032E5F84}"/>
   </bookViews>
@@ -791,90 +791,90 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
@@ -1236,7 +1236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07BC9FE6-99F2-45D8-A543-7E369AECEF65}">
   <dimension ref="A1:CD40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -1259,11 +1259,11 @@
     <col min="18" max="18" width="12.21875" style="57" customWidth="1"/>
     <col min="19" max="19" width="7.44140625" style="9" customWidth="1"/>
     <col min="20" max="20" width="5.21875" style="9" customWidth="1"/>
-    <col min="21" max="21" width="11" style="57" customWidth="1"/>
+    <col min="21" max="21" width="13.21875" style="57" customWidth="1"/>
     <col min="22" max="22" width="8" style="9" customWidth="1"/>
     <col min="23" max="24" width="8.21875" style="9" customWidth="1"/>
     <col min="25" max="25" width="8.44140625" style="9" customWidth="1"/>
-    <col min="26" max="26" width="10.33203125" style="57" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.5546875" style="57" customWidth="1"/>
     <col min="27" max="27" width="9.44140625" style="9" customWidth="1"/>
     <col min="28" max="28" width="8.21875" style="9" customWidth="1"/>
     <col min="29" max="29" width="7.77734375" style="9" customWidth="1"/>
@@ -1275,12 +1275,12 @@
     <col min="35" max="35" width="8.109375" customWidth="1"/>
     <col min="36" max="36" width="13" customWidth="1"/>
     <col min="37" max="38" width="6.77734375" customWidth="1"/>
-    <col min="39" max="39" width="9.21875" customWidth="1"/>
+    <col min="39" max="39" width="13.5546875" customWidth="1"/>
     <col min="40" max="40" width="7" style="9" customWidth="1"/>
     <col min="41" max="43" width="6.5546875" style="9" customWidth="1"/>
     <col min="44" max="44" width="9.109375" style="9" customWidth="1"/>
     <col min="45" max="48" width="6.5546875" style="9" customWidth="1"/>
-    <col min="49" max="49" width="8.109375" style="9" customWidth="1"/>
+    <col min="49" max="49" width="14.109375" style="9" customWidth="1"/>
     <col min="50" max="53" width="6.5546875" style="9" customWidth="1"/>
     <col min="54" max="54" width="9.77734375" style="9" customWidth="1"/>
     <col min="55" max="55" width="7.77734375" style="9" customWidth="1"/>
@@ -1290,255 +1290,255 @@
     <col min="59" max="59" width="10.88671875" style="9" customWidth="1"/>
     <col min="60" max="60" width="9.77734375" style="9" customWidth="1"/>
     <col min="61" max="61" width="7.21875" style="9" customWidth="1"/>
-    <col min="62" max="62" width="8.88671875" style="9" customWidth="1"/>
+    <col min="62" max="62" width="14.33203125" style="9" customWidth="1"/>
     <col min="63" max="66" width="7.21875" style="9" customWidth="1"/>
-    <col min="67" max="67" width="11.33203125" style="9" customWidth="1"/>
+    <col min="67" max="67" width="13.5546875" style="9" customWidth="1"/>
     <col min="68" max="71" width="7.21875" style="9" customWidth="1"/>
-    <col min="72" max="72" width="9.88671875" style="9" customWidth="1"/>
+    <col min="72" max="72" width="14.77734375" style="9" customWidth="1"/>
     <col min="73" max="73" width="10" style="9" customWidth="1"/>
     <col min="74" max="74" width="9.44140625" style="9" customWidth="1"/>
-    <col min="75" max="75" width="12.109375" style="9" customWidth="1"/>
+    <col min="75" max="75" width="17.21875" style="9" customWidth="1"/>
     <col min="76" max="79" width="7.21875" customWidth="1"/>
     <col min="80" max="80" width="11.77734375" customWidth="1"/>
     <col min="81" max="81" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:82" s="1" customFormat="1" ht="21">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="73"/>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="73"/>
-      <c r="S1" s="73"/>
-      <c r="T1" s="73"/>
-      <c r="U1" s="73"/>
-      <c r="V1" s="73"/>
-      <c r="W1" s="73"/>
-      <c r="X1" s="73"/>
-      <c r="Y1" s="73"/>
-      <c r="Z1" s="73"/>
-      <c r="AA1" s="73"/>
-      <c r="AB1" s="73"/>
-      <c r="AC1" s="73"/>
-      <c r="AD1" s="73"/>
-      <c r="AE1" s="73"/>
-      <c r="AF1" s="73"/>
-      <c r="AG1" s="73"/>
-      <c r="AH1" s="73"/>
-      <c r="AI1" s="73"/>
-      <c r="AJ1" s="73"/>
-      <c r="AK1" s="73"/>
-      <c r="AL1" s="73"/>
-      <c r="AM1" s="73"/>
-      <c r="AN1" s="73"/>
-      <c r="AO1" s="73"/>
-      <c r="AP1" s="73"/>
-      <c r="AQ1" s="73"/>
-      <c r="AR1" s="73"/>
-      <c r="AS1" s="73"/>
-      <c r="AT1" s="73"/>
-      <c r="AU1" s="73"/>
-      <c r="AV1" s="73"/>
-      <c r="AW1" s="73"/>
-      <c r="AX1" s="73"/>
-      <c r="AY1" s="73"/>
-      <c r="AZ1" s="73"/>
-      <c r="BA1" s="73"/>
-      <c r="BB1" s="73"/>
-      <c r="BC1" s="73"/>
-      <c r="BD1" s="73"/>
-      <c r="BE1" s="73"/>
-      <c r="BF1" s="73"/>
-      <c r="BG1" s="73"/>
-      <c r="BH1" s="73"/>
-      <c r="BI1" s="73"/>
-      <c r="BJ1" s="73"/>
-      <c r="BK1" s="73"/>
-      <c r="BL1" s="73"/>
-      <c r="BM1" s="73"/>
-      <c r="BN1" s="73"/>
-      <c r="BO1" s="73"/>
-      <c r="BP1" s="73"/>
-      <c r="BQ1" s="73"/>
-      <c r="BR1" s="73"/>
-      <c r="BS1" s="73"/>
-      <c r="BT1" s="73"/>
-      <c r="BU1" s="73"/>
-      <c r="BV1" s="73"/>
-      <c r="BW1" s="73"/>
-      <c r="BX1" s="73"/>
-      <c r="BY1" s="73"/>
-      <c r="BZ1" s="73"/>
-      <c r="CA1" s="73"/>
-      <c r="CB1" s="73"/>
-      <c r="CC1" s="73"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="96"/>
+      <c r="O1" s="96"/>
+      <c r="P1" s="96"/>
+      <c r="Q1" s="96"/>
+      <c r="R1" s="96"/>
+      <c r="S1" s="96"/>
+      <c r="T1" s="96"/>
+      <c r="U1" s="96"/>
+      <c r="V1" s="96"/>
+      <c r="W1" s="96"/>
+      <c r="X1" s="96"/>
+      <c r="Y1" s="96"/>
+      <c r="Z1" s="96"/>
+      <c r="AA1" s="96"/>
+      <c r="AB1" s="96"/>
+      <c r="AC1" s="96"/>
+      <c r="AD1" s="96"/>
+      <c r="AE1" s="96"/>
+      <c r="AF1" s="96"/>
+      <c r="AG1" s="96"/>
+      <c r="AH1" s="96"/>
+      <c r="AI1" s="96"/>
+      <c r="AJ1" s="96"/>
+      <c r="AK1" s="96"/>
+      <c r="AL1" s="96"/>
+      <c r="AM1" s="96"/>
+      <c r="AN1" s="96"/>
+      <c r="AO1" s="96"/>
+      <c r="AP1" s="96"/>
+      <c r="AQ1" s="96"/>
+      <c r="AR1" s="96"/>
+      <c r="AS1" s="96"/>
+      <c r="AT1" s="96"/>
+      <c r="AU1" s="96"/>
+      <c r="AV1" s="96"/>
+      <c r="AW1" s="96"/>
+      <c r="AX1" s="96"/>
+      <c r="AY1" s="96"/>
+      <c r="AZ1" s="96"/>
+      <c r="BA1" s="96"/>
+      <c r="BB1" s="96"/>
+      <c r="BC1" s="96"/>
+      <c r="BD1" s="96"/>
+      <c r="BE1" s="96"/>
+      <c r="BF1" s="96"/>
+      <c r="BG1" s="96"/>
+      <c r="BH1" s="96"/>
+      <c r="BI1" s="96"/>
+      <c r="BJ1" s="96"/>
+      <c r="BK1" s="96"/>
+      <c r="BL1" s="96"/>
+      <c r="BM1" s="96"/>
+      <c r="BN1" s="96"/>
+      <c r="BO1" s="96"/>
+      <c r="BP1" s="96"/>
+      <c r="BQ1" s="96"/>
+      <c r="BR1" s="96"/>
+      <c r="BS1" s="96"/>
+      <c r="BT1" s="96"/>
+      <c r="BU1" s="96"/>
+      <c r="BV1" s="96"/>
+      <c r="BW1" s="96"/>
+      <c r="BX1" s="96"/>
+      <c r="BY1" s="96"/>
+      <c r="BZ1" s="96"/>
+      <c r="CA1" s="96"/>
+      <c r="CB1" s="96"/>
+      <c r="CC1" s="96"/>
     </row>
     <row r="2" spans="1:82" s="1" customFormat="1" ht="21">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="96" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
-      <c r="S2" s="73"/>
-      <c r="T2" s="73"/>
-      <c r="U2" s="73"/>
-      <c r="V2" s="73"/>
-      <c r="W2" s="73"/>
-      <c r="X2" s="73"/>
-      <c r="Y2" s="73"/>
-      <c r="Z2" s="73"/>
-      <c r="AA2" s="73"/>
-      <c r="AB2" s="73"/>
-      <c r="AC2" s="73"/>
-      <c r="AD2" s="73"/>
-      <c r="AE2" s="73"/>
-      <c r="AF2" s="73"/>
-      <c r="AG2" s="73"/>
-      <c r="AH2" s="73"/>
-      <c r="AI2" s="73"/>
-      <c r="AJ2" s="73"/>
-      <c r="AK2" s="73"/>
-      <c r="AL2" s="73"/>
-      <c r="AM2" s="73"/>
-      <c r="AN2" s="73"/>
-      <c r="AO2" s="73"/>
-      <c r="AP2" s="73"/>
-      <c r="AQ2" s="73"/>
-      <c r="AR2" s="73"/>
-      <c r="AS2" s="73"/>
-      <c r="AT2" s="73"/>
-      <c r="AU2" s="73"/>
-      <c r="AV2" s="73"/>
-      <c r="AW2" s="73"/>
-      <c r="AX2" s="73"/>
-      <c r="AY2" s="73"/>
-      <c r="AZ2" s="73"/>
-      <c r="BA2" s="73"/>
-      <c r="BB2" s="73"/>
-      <c r="BC2" s="73"/>
-      <c r="BD2" s="73"/>
-      <c r="BE2" s="73"/>
-      <c r="BF2" s="73"/>
-      <c r="BG2" s="73"/>
-      <c r="BH2" s="73"/>
-      <c r="BI2" s="73"/>
-      <c r="BJ2" s="73"/>
-      <c r="BK2" s="73"/>
-      <c r="BL2" s="73"/>
-      <c r="BM2" s="73"/>
-      <c r="BN2" s="73"/>
-      <c r="BO2" s="73"/>
-      <c r="BP2" s="73"/>
-      <c r="BQ2" s="73"/>
-      <c r="BR2" s="73"/>
-      <c r="BS2" s="73"/>
-      <c r="BT2" s="73"/>
-      <c r="BU2" s="73"/>
-      <c r="BV2" s="73"/>
-      <c r="BW2" s="73"/>
-      <c r="BX2" s="73"/>
-      <c r="BY2" s="73"/>
-      <c r="BZ2" s="73"/>
-      <c r="CA2" s="73"/>
-      <c r="CB2" s="73"/>
-      <c r="CC2" s="73"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="96"/>
+      <c r="P2" s="96"/>
+      <c r="Q2" s="96"/>
+      <c r="R2" s="96"/>
+      <c r="S2" s="96"/>
+      <c r="T2" s="96"/>
+      <c r="U2" s="96"/>
+      <c r="V2" s="96"/>
+      <c r="W2" s="96"/>
+      <c r="X2" s="96"/>
+      <c r="Y2" s="96"/>
+      <c r="Z2" s="96"/>
+      <c r="AA2" s="96"/>
+      <c r="AB2" s="96"/>
+      <c r="AC2" s="96"/>
+      <c r="AD2" s="96"/>
+      <c r="AE2" s="96"/>
+      <c r="AF2" s="96"/>
+      <c r="AG2" s="96"/>
+      <c r="AH2" s="96"/>
+      <c r="AI2" s="96"/>
+      <c r="AJ2" s="96"/>
+      <c r="AK2" s="96"/>
+      <c r="AL2" s="96"/>
+      <c r="AM2" s="96"/>
+      <c r="AN2" s="96"/>
+      <c r="AO2" s="96"/>
+      <c r="AP2" s="96"/>
+      <c r="AQ2" s="96"/>
+      <c r="AR2" s="96"/>
+      <c r="AS2" s="96"/>
+      <c r="AT2" s="96"/>
+      <c r="AU2" s="96"/>
+      <c r="AV2" s="96"/>
+      <c r="AW2" s="96"/>
+      <c r="AX2" s="96"/>
+      <c r="AY2" s="96"/>
+      <c r="AZ2" s="96"/>
+      <c r="BA2" s="96"/>
+      <c r="BB2" s="96"/>
+      <c r="BC2" s="96"/>
+      <c r="BD2" s="96"/>
+      <c r="BE2" s="96"/>
+      <c r="BF2" s="96"/>
+      <c r="BG2" s="96"/>
+      <c r="BH2" s="96"/>
+      <c r="BI2" s="96"/>
+      <c r="BJ2" s="96"/>
+      <c r="BK2" s="96"/>
+      <c r="BL2" s="96"/>
+      <c r="BM2" s="96"/>
+      <c r="BN2" s="96"/>
+      <c r="BO2" s="96"/>
+      <c r="BP2" s="96"/>
+      <c r="BQ2" s="96"/>
+      <c r="BR2" s="96"/>
+      <c r="BS2" s="96"/>
+      <c r="BT2" s="96"/>
+      <c r="BU2" s="96"/>
+      <c r="BV2" s="96"/>
+      <c r="BW2" s="96"/>
+      <c r="BX2" s="96"/>
+      <c r="BY2" s="96"/>
+      <c r="BZ2" s="96"/>
+      <c r="CA2" s="96"/>
+      <c r="CB2" s="96"/>
+      <c r="CC2" s="96"/>
     </row>
     <row r="4" spans="1:82" s="4" customFormat="1" ht="29.1" customHeight="1">
-      <c r="A4" s="74" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="86" t="s">
+      <c r="A4" s="87" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="86" t="s">
+      <c r="C4" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="92" t="s">
+      <c r="D4" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="93"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="93"/>
-      <c r="H4" s="93"/>
-      <c r="I4" s="93"/>
-      <c r="J4" s="93"/>
-      <c r="K4" s="93"/>
-      <c r="L4" s="93"/>
-      <c r="M4" s="93"/>
-      <c r="N4" s="93"/>
-      <c r="O4" s="93"/>
-      <c r="P4" s="93"/>
-      <c r="Q4" s="93"/>
-      <c r="R4" s="93"/>
-      <c r="S4" s="93"/>
-      <c r="T4" s="93"/>
-      <c r="U4" s="93"/>
-      <c r="V4" s="93"/>
-      <c r="W4" s="93"/>
-      <c r="X4" s="93"/>
-      <c r="Y4" s="93"/>
-      <c r="Z4" s="93"/>
-      <c r="AA4" s="93"/>
-      <c r="AB4" s="93"/>
-      <c r="AC4" s="93"/>
-      <c r="AD4" s="93"/>
-      <c r="AE4" s="93"/>
-      <c r="AF4" s="93"/>
-      <c r="AG4" s="93"/>
-      <c r="AH4" s="93"/>
-      <c r="AI4" s="93"/>
-      <c r="AJ4" s="93"/>
-      <c r="AK4" s="93"/>
-      <c r="AL4" s="93"/>
-      <c r="AM4" s="93"/>
-      <c r="AN4" s="93"/>
-      <c r="AO4" s="93"/>
-      <c r="AP4" s="93"/>
-      <c r="AQ4" s="93"/>
-      <c r="AR4" s="93"/>
-      <c r="AS4" s="93"/>
-      <c r="AT4" s="93"/>
-      <c r="AU4" s="93"/>
-      <c r="AV4" s="93"/>
-      <c r="AW4" s="93"/>
-      <c r="AX4" s="93"/>
-      <c r="AY4" s="93"/>
-      <c r="AZ4" s="93"/>
-      <c r="BA4" s="93"/>
-      <c r="BB4" s="93"/>
-      <c r="BC4" s="93"/>
-      <c r="BD4" s="93"/>
-      <c r="BE4" s="93"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="80"/>
+      <c r="K4" s="80"/>
+      <c r="L4" s="80"/>
+      <c r="M4" s="80"/>
+      <c r="N4" s="80"/>
+      <c r="O4" s="80"/>
+      <c r="P4" s="80"/>
+      <c r="Q4" s="80"/>
+      <c r="R4" s="80"/>
+      <c r="S4" s="80"/>
+      <c r="T4" s="80"/>
+      <c r="U4" s="80"/>
+      <c r="V4" s="80"/>
+      <c r="W4" s="80"/>
+      <c r="X4" s="80"/>
+      <c r="Y4" s="80"/>
+      <c r="Z4" s="80"/>
+      <c r="AA4" s="80"/>
+      <c r="AB4" s="80"/>
+      <c r="AC4" s="80"/>
+      <c r="AD4" s="80"/>
+      <c r="AE4" s="80"/>
+      <c r="AF4" s="80"/>
+      <c r="AG4" s="80"/>
+      <c r="AH4" s="80"/>
+      <c r="AI4" s="80"/>
+      <c r="AJ4" s="80"/>
+      <c r="AK4" s="80"/>
+      <c r="AL4" s="80"/>
+      <c r="AM4" s="80"/>
+      <c r="AN4" s="80"/>
+      <c r="AO4" s="80"/>
+      <c r="AP4" s="80"/>
+      <c r="AQ4" s="80"/>
+      <c r="AR4" s="80"/>
+      <c r="AS4" s="80"/>
+      <c r="AT4" s="80"/>
+      <c r="AU4" s="80"/>
+      <c r="AV4" s="80"/>
+      <c r="AW4" s="80"/>
+      <c r="AX4" s="80"/>
+      <c r="AY4" s="80"/>
+      <c r="AZ4" s="80"/>
+      <c r="BA4" s="80"/>
+      <c r="BB4" s="80"/>
+      <c r="BC4" s="80"/>
+      <c r="BD4" s="80"/>
+      <c r="BE4" s="80"/>
       <c r="BF4" s="12"/>
       <c r="BG4" s="12"/>
       <c r="BH4" s="12"/>
@@ -1557,416 +1557,416 @@
       <c r="BU4" s="12"/>
       <c r="BV4" s="12"/>
       <c r="BW4" s="12"/>
-      <c r="BX4" s="79" t="s">
+      <c r="BX4" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="BY4" s="80"/>
-      <c r="BZ4" s="80"/>
-      <c r="CA4" s="81"/>
-      <c r="CB4" s="70" t="s">
+      <c r="BY4" s="71"/>
+      <c r="BZ4" s="71"/>
+      <c r="CA4" s="72"/>
+      <c r="CB4" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="CC4" s="70" t="s">
+      <c r="CC4" s="93" t="s">
         <v>5</v>
       </c>
       <c r="CD4" s="3"/>
     </row>
     <row r="5" spans="1:82" s="4" customFormat="1" ht="21.6" customHeight="1">
-      <c r="A5" s="85"/>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="78" t="s">
+      <c r="A5" s="89"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="78"/>
-      <c r="M5" s="78"/>
-      <c r="N5" s="78"/>
-      <c r="O5" s="78"/>
-      <c r="P5" s="78"/>
-      <c r="Q5" s="78"/>
-      <c r="R5" s="78"/>
-      <c r="S5" s="79" t="s">
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="81"/>
+      <c r="K5" s="81"/>
+      <c r="L5" s="81"/>
+      <c r="M5" s="81"/>
+      <c r="N5" s="81"/>
+      <c r="O5" s="81"/>
+      <c r="P5" s="81"/>
+      <c r="Q5" s="81"/>
+      <c r="R5" s="81"/>
+      <c r="S5" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="T5" s="80"/>
-      <c r="U5" s="81"/>
-      <c r="V5" s="78" t="s">
+      <c r="T5" s="71"/>
+      <c r="U5" s="72"/>
+      <c r="V5" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="W5" s="78"/>
-      <c r="X5" s="78"/>
-      <c r="Y5" s="78"/>
-      <c r="Z5" s="78"/>
-      <c r="AA5" s="78"/>
-      <c r="AB5" s="78"/>
-      <c r="AC5" s="78"/>
-      <c r="AD5" s="78"/>
-      <c r="AE5" s="78"/>
-      <c r="AF5" s="78"/>
-      <c r="AG5" s="78"/>
-      <c r="AH5" s="78"/>
-      <c r="AI5" s="78"/>
-      <c r="AJ5" s="78"/>
-      <c r="AK5" s="79" t="s">
+      <c r="W5" s="81"/>
+      <c r="X5" s="81"/>
+      <c r="Y5" s="81"/>
+      <c r="Z5" s="81"/>
+      <c r="AA5" s="81"/>
+      <c r="AB5" s="81"/>
+      <c r="AC5" s="81"/>
+      <c r="AD5" s="81"/>
+      <c r="AE5" s="81"/>
+      <c r="AF5" s="81"/>
+      <c r="AG5" s="81"/>
+      <c r="AH5" s="81"/>
+      <c r="AI5" s="81"/>
+      <c r="AJ5" s="81"/>
+      <c r="AK5" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="AL5" s="80"/>
-      <c r="AM5" s="81"/>
-      <c r="AN5" s="78" t="s">
+      <c r="AL5" s="71"/>
+      <c r="AM5" s="72"/>
+      <c r="AN5" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="AO5" s="78"/>
-      <c r="AP5" s="78"/>
-      <c r="AQ5" s="78"/>
-      <c r="AR5" s="78"/>
-      <c r="AS5" s="78"/>
-      <c r="AT5" s="78"/>
-      <c r="AU5" s="78"/>
-      <c r="AV5" s="78"/>
-      <c r="AW5" s="78"/>
-      <c r="AX5" s="78"/>
-      <c r="AY5" s="78"/>
-      <c r="AZ5" s="78"/>
-      <c r="BA5" s="78"/>
-      <c r="BB5" s="78"/>
-      <c r="BC5" s="79" t="s">
+      <c r="AO5" s="81"/>
+      <c r="AP5" s="81"/>
+      <c r="AQ5" s="81"/>
+      <c r="AR5" s="81"/>
+      <c r="AS5" s="81"/>
+      <c r="AT5" s="81"/>
+      <c r="AU5" s="81"/>
+      <c r="AV5" s="81"/>
+      <c r="AW5" s="81"/>
+      <c r="AX5" s="81"/>
+      <c r="AY5" s="81"/>
+      <c r="AZ5" s="81"/>
+      <c r="BA5" s="81"/>
+      <c r="BB5" s="81"/>
+      <c r="BC5" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="BD5" s="80"/>
-      <c r="BE5" s="81"/>
-      <c r="BF5" s="78" t="s">
+      <c r="BD5" s="71"/>
+      <c r="BE5" s="72"/>
+      <c r="BF5" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="BG5" s="78"/>
-      <c r="BH5" s="78"/>
-      <c r="BI5" s="78"/>
-      <c r="BJ5" s="78"/>
-      <c r="BK5" s="78"/>
-      <c r="BL5" s="78"/>
-      <c r="BM5" s="78"/>
-      <c r="BN5" s="78"/>
-      <c r="BO5" s="78"/>
-      <c r="BP5" s="78"/>
-      <c r="BQ5" s="78"/>
-      <c r="BR5" s="78"/>
-      <c r="BS5" s="78"/>
-      <c r="BT5" s="78"/>
-      <c r="BU5" s="79" t="s">
+      <c r="BG5" s="81"/>
+      <c r="BH5" s="81"/>
+      <c r="BI5" s="81"/>
+      <c r="BJ5" s="81"/>
+      <c r="BK5" s="81"/>
+      <c r="BL5" s="81"/>
+      <c r="BM5" s="81"/>
+      <c r="BN5" s="81"/>
+      <c r="BO5" s="81"/>
+      <c r="BP5" s="81"/>
+      <c r="BQ5" s="81"/>
+      <c r="BR5" s="81"/>
+      <c r="BS5" s="81"/>
+      <c r="BT5" s="81"/>
+      <c r="BU5" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="BV5" s="80"/>
-      <c r="BW5" s="81"/>
-      <c r="BX5" s="89"/>
-      <c r="BY5" s="90"/>
-      <c r="BZ5" s="90"/>
-      <c r="CA5" s="91"/>
-      <c r="CB5" s="71"/>
-      <c r="CC5" s="71"/>
+      <c r="BV5" s="71"/>
+      <c r="BW5" s="72"/>
+      <c r="BX5" s="73"/>
+      <c r="BY5" s="74"/>
+      <c r="BZ5" s="74"/>
+      <c r="CA5" s="75"/>
+      <c r="CB5" s="94"/>
+      <c r="CC5" s="94"/>
       <c r="CD5" s="3"/>
     </row>
     <row r="6" spans="1:82" s="4" customFormat="1" ht="21.6" customHeight="1">
-      <c r="A6" s="85"/>
-      <c r="B6" s="87"/>
-      <c r="C6" s="87"/>
-      <c r="D6" s="78" t="s">
+      <c r="A6" s="89"/>
+      <c r="B6" s="91"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="78" t="s">
+      <c r="E6" s="81"/>
+      <c r="F6" s="81"/>
+      <c r="G6" s="81"/>
+      <c r="H6" s="81"/>
+      <c r="I6" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
-      <c r="L6" s="68"/>
-      <c r="M6" s="69"/>
-      <c r="N6" s="78" t="s">
+      <c r="J6" s="82"/>
+      <c r="K6" s="82"/>
+      <c r="L6" s="82"/>
+      <c r="M6" s="83"/>
+      <c r="N6" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="O6" s="68"/>
-      <c r="P6" s="68"/>
-      <c r="Q6" s="68"/>
-      <c r="R6" s="69"/>
-      <c r="S6" s="82"/>
-      <c r="T6" s="83"/>
-      <c r="U6" s="84"/>
-      <c r="V6" s="78" t="s">
+      <c r="O6" s="82"/>
+      <c r="P6" s="82"/>
+      <c r="Q6" s="82"/>
+      <c r="R6" s="83"/>
+      <c r="S6" s="76"/>
+      <c r="T6" s="77"/>
+      <c r="U6" s="78"/>
+      <c r="V6" s="81" t="s">
         <v>17</v>
       </c>
-      <c r="W6" s="78"/>
-      <c r="X6" s="78"/>
-      <c r="Y6" s="78"/>
-      <c r="Z6" s="78"/>
-      <c r="AA6" s="78" t="s">
+      <c r="W6" s="81"/>
+      <c r="X6" s="81"/>
+      <c r="Y6" s="81"/>
+      <c r="Z6" s="81"/>
+      <c r="AA6" s="81" t="s">
         <v>18</v>
       </c>
-      <c r="AB6" s="68"/>
-      <c r="AC6" s="68"/>
-      <c r="AD6" s="68"/>
-      <c r="AE6" s="69"/>
-      <c r="AF6" s="78" t="s">
+      <c r="AB6" s="82"/>
+      <c r="AC6" s="82"/>
+      <c r="AD6" s="82"/>
+      <c r="AE6" s="83"/>
+      <c r="AF6" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="AG6" s="68"/>
-      <c r="AH6" s="68"/>
-      <c r="AI6" s="68"/>
-      <c r="AJ6" s="69"/>
-      <c r="AK6" s="82"/>
-      <c r="AL6" s="83"/>
-      <c r="AM6" s="84"/>
-      <c r="AN6" s="78" t="s">
+      <c r="AG6" s="82"/>
+      <c r="AH6" s="82"/>
+      <c r="AI6" s="82"/>
+      <c r="AJ6" s="83"/>
+      <c r="AK6" s="76"/>
+      <c r="AL6" s="77"/>
+      <c r="AM6" s="78"/>
+      <c r="AN6" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="AO6" s="78"/>
-      <c r="AP6" s="78"/>
-      <c r="AQ6" s="78"/>
-      <c r="AR6" s="78"/>
-      <c r="AS6" s="78" t="s">
+      <c r="AO6" s="81"/>
+      <c r="AP6" s="81"/>
+      <c r="AQ6" s="81"/>
+      <c r="AR6" s="81"/>
+      <c r="AS6" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="AT6" s="68"/>
-      <c r="AU6" s="68"/>
-      <c r="AV6" s="68"/>
-      <c r="AW6" s="69"/>
-      <c r="AX6" s="78" t="s">
+      <c r="AT6" s="82"/>
+      <c r="AU6" s="82"/>
+      <c r="AV6" s="82"/>
+      <c r="AW6" s="83"/>
+      <c r="AX6" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="AY6" s="68"/>
-      <c r="AZ6" s="68"/>
-      <c r="BA6" s="68"/>
-      <c r="BB6" s="69"/>
-      <c r="BC6" s="82"/>
-      <c r="BD6" s="83"/>
-      <c r="BE6" s="84"/>
-      <c r="BF6" s="78" t="s">
+      <c r="AY6" s="82"/>
+      <c r="AZ6" s="82"/>
+      <c r="BA6" s="82"/>
+      <c r="BB6" s="83"/>
+      <c r="BC6" s="76"/>
+      <c r="BD6" s="77"/>
+      <c r="BE6" s="78"/>
+      <c r="BF6" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="BG6" s="78"/>
-      <c r="BH6" s="78"/>
-      <c r="BI6" s="78"/>
-      <c r="BJ6" s="78"/>
-      <c r="BK6" s="78" t="s">
+      <c r="BG6" s="81"/>
+      <c r="BH6" s="81"/>
+      <c r="BI6" s="81"/>
+      <c r="BJ6" s="81"/>
+      <c r="BK6" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="BL6" s="68"/>
-      <c r="BM6" s="68"/>
-      <c r="BN6" s="68"/>
-      <c r="BO6" s="69"/>
-      <c r="BP6" s="78" t="s">
+      <c r="BL6" s="82"/>
+      <c r="BM6" s="82"/>
+      <c r="BN6" s="82"/>
+      <c r="BO6" s="83"/>
+      <c r="BP6" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="BQ6" s="68"/>
-      <c r="BR6" s="68"/>
-      <c r="BS6" s="68"/>
-      <c r="BT6" s="69"/>
-      <c r="BU6" s="82"/>
-      <c r="BV6" s="83"/>
-      <c r="BW6" s="84"/>
-      <c r="BX6" s="82"/>
-      <c r="BY6" s="83"/>
-      <c r="BZ6" s="83"/>
-      <c r="CA6" s="84"/>
-      <c r="CB6" s="71"/>
-      <c r="CC6" s="71"/>
+      <c r="BQ6" s="82"/>
+      <c r="BR6" s="82"/>
+      <c r="BS6" s="82"/>
+      <c r="BT6" s="83"/>
+      <c r="BU6" s="76"/>
+      <c r="BV6" s="77"/>
+      <c r="BW6" s="78"/>
+      <c r="BX6" s="76"/>
+      <c r="BY6" s="77"/>
+      <c r="BZ6" s="77"/>
+      <c r="CA6" s="78"/>
+      <c r="CB6" s="94"/>
+      <c r="CC6" s="94"/>
       <c r="CD6" s="3"/>
     </row>
     <row r="7" spans="1:82" s="4" customFormat="1" ht="21.6" customHeight="1">
-      <c r="A7" s="85"/>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="67" t="s">
+      <c r="A7" s="89"/>
+      <c r="B7" s="91"/>
+      <c r="C7" s="91"/>
+      <c r="D7" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="74" t="s">
+      <c r="E7" s="82"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="76" t="s">
+      <c r="H7" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="67" t="s">
+      <c r="I7" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="68"/>
-      <c r="K7" s="69"/>
-      <c r="L7" s="74" t="s">
+      <c r="J7" s="82"/>
+      <c r="K7" s="83"/>
+      <c r="L7" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="M7" s="76" t="s">
+      <c r="M7" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="N7" s="67" t="s">
+      <c r="N7" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="O7" s="68"/>
-      <c r="P7" s="69"/>
-      <c r="Q7" s="76" t="s">
+      <c r="O7" s="82"/>
+      <c r="P7" s="83"/>
+      <c r="Q7" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="R7" s="76" t="s">
+      <c r="R7" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="S7" s="74" t="s">
+      <c r="S7" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="T7" s="74" t="s">
+      <c r="T7" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="U7" s="76" t="s">
+      <c r="U7" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="V7" s="67" t="s">
+      <c r="V7" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="W7" s="68"/>
-      <c r="X7" s="69"/>
-      <c r="Y7" s="74" t="s">
+      <c r="W7" s="82"/>
+      <c r="X7" s="83"/>
+      <c r="Y7" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="Z7" s="76" t="s">
+      <c r="Z7" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="AA7" s="67" t="s">
+      <c r="AA7" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="AB7" s="68"/>
-      <c r="AC7" s="69"/>
-      <c r="AD7" s="74" t="s">
+      <c r="AB7" s="82"/>
+      <c r="AC7" s="83"/>
+      <c r="AD7" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="AE7" s="76" t="s">
+      <c r="AE7" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="AF7" s="67" t="s">
+      <c r="AF7" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="AG7" s="68"/>
-      <c r="AH7" s="69"/>
-      <c r="AI7" s="74" t="s">
+      <c r="AG7" s="82"/>
+      <c r="AH7" s="83"/>
+      <c r="AI7" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="AJ7" s="76" t="s">
+      <c r="AJ7" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="AK7" s="74" t="s">
+      <c r="AK7" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="AL7" s="74" t="s">
+      <c r="AL7" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="AM7" s="76" t="s">
+      <c r="AM7" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="AN7" s="67" t="s">
+      <c r="AN7" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="AO7" s="68"/>
-      <c r="AP7" s="69"/>
-      <c r="AQ7" s="74" t="s">
+      <c r="AO7" s="82"/>
+      <c r="AP7" s="83"/>
+      <c r="AQ7" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="AR7" s="76" t="s">
+      <c r="AR7" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="AS7" s="67" t="s">
+      <c r="AS7" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="AT7" s="68"/>
-      <c r="AU7" s="69"/>
-      <c r="AV7" s="74" t="s">
+      <c r="AT7" s="82"/>
+      <c r="AU7" s="83"/>
+      <c r="AV7" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="AW7" s="76" t="s">
+      <c r="AW7" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="AX7" s="67" t="s">
+      <c r="AX7" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="AY7" s="68"/>
-      <c r="AZ7" s="69"/>
-      <c r="BA7" s="74" t="s">
+      <c r="AY7" s="82"/>
+      <c r="AZ7" s="83"/>
+      <c r="BA7" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="BB7" s="76" t="s">
+      <c r="BB7" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="BC7" s="74" t="s">
+      <c r="BC7" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="BD7" s="74" t="s">
+      <c r="BD7" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="BE7" s="76" t="s">
+      <c r="BE7" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="BF7" s="67" t="s">
+      <c r="BF7" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="BG7" s="68"/>
-      <c r="BH7" s="69"/>
-      <c r="BI7" s="74" t="s">
+      <c r="BG7" s="82"/>
+      <c r="BH7" s="83"/>
+      <c r="BI7" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="BJ7" s="76" t="s">
+      <c r="BJ7" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="BK7" s="67" t="s">
+      <c r="BK7" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="BL7" s="68"/>
-      <c r="BM7" s="69"/>
-      <c r="BN7" s="74" t="s">
+      <c r="BL7" s="82"/>
+      <c r="BM7" s="83"/>
+      <c r="BN7" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="BO7" s="76" t="s">
+      <c r="BO7" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="BP7" s="67" t="s">
+      <c r="BP7" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="BQ7" s="68"/>
-      <c r="BR7" s="69"/>
-      <c r="BS7" s="74" t="s">
+      <c r="BQ7" s="82"/>
+      <c r="BR7" s="83"/>
+      <c r="BS7" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="BT7" s="76" t="s">
+      <c r="BT7" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="BU7" s="74" t="s">
+      <c r="BU7" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="BV7" s="74" t="s">
+      <c r="BV7" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="BW7" s="74" t="s">
+      <c r="BW7" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="BX7" s="67" t="s">
+      <c r="BX7" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="BY7" s="68"/>
-      <c r="BZ7" s="69"/>
-      <c r="CA7" s="74" t="s">
+      <c r="BY7" s="82"/>
+      <c r="BZ7" s="83"/>
+      <c r="CA7" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="CB7" s="71"/>
-      <c r="CC7" s="71"/>
+      <c r="CB7" s="94"/>
+      <c r="CC7" s="94"/>
       <c r="CD7" s="3"/>
     </row>
     <row r="8" spans="1:82" s="4" customFormat="1" ht="21.6" customHeight="1">
-      <c r="A8" s="75"/>
-      <c r="B8" s="88"/>
-      <c r="C8" s="88"/>
+      <c r="A8" s="88"/>
+      <c r="B8" s="92"/>
+      <c r="C8" s="92"/>
       <c r="D8" s="2" t="s">
         <v>31</v>
       </c>
@@ -1976,8 +1976,8 @@
       <c r="F8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="75"/>
-      <c r="H8" s="77"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="86"/>
       <c r="I8" s="2" t="s">
         <v>31</v>
       </c>
@@ -1987,8 +1987,8 @@
       <c r="K8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L8" s="75"/>
-      <c r="M8" s="77"/>
+      <c r="L8" s="88"/>
+      <c r="M8" s="86"/>
       <c r="N8" s="2" t="s">
         <v>31</v>
       </c>
@@ -1998,11 +1998,11 @@
       <c r="P8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="Q8" s="77"/>
-      <c r="R8" s="77"/>
-      <c r="S8" s="75"/>
-      <c r="T8" s="75"/>
-      <c r="U8" s="77"/>
+      <c r="Q8" s="86"/>
+      <c r="R8" s="86"/>
+      <c r="S8" s="88"/>
+      <c r="T8" s="88"/>
+      <c r="U8" s="86"/>
       <c r="V8" s="2" t="s">
         <v>31</v>
       </c>
@@ -2012,8 +2012,8 @@
       <c r="X8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="Y8" s="75"/>
-      <c r="Z8" s="77"/>
+      <c r="Y8" s="88"/>
+      <c r="Z8" s="86"/>
       <c r="AA8" s="2" t="s">
         <v>31</v>
       </c>
@@ -2023,8 +2023,8 @@
       <c r="AC8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD8" s="75"/>
-      <c r="AE8" s="77"/>
+      <c r="AD8" s="88"/>
+      <c r="AE8" s="86"/>
       <c r="AF8" s="2" t="s">
         <v>31</v>
       </c>
@@ -2034,11 +2034,11 @@
       <c r="AH8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AI8" s="75"/>
-      <c r="AJ8" s="77"/>
-      <c r="AK8" s="75"/>
-      <c r="AL8" s="75"/>
-      <c r="AM8" s="77"/>
+      <c r="AI8" s="88"/>
+      <c r="AJ8" s="86"/>
+      <c r="AK8" s="88"/>
+      <c r="AL8" s="88"/>
+      <c r="AM8" s="86"/>
       <c r="AN8" s="2" t="s">
         <v>31</v>
       </c>
@@ -2048,8 +2048,8 @@
       <c r="AP8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AQ8" s="75"/>
-      <c r="AR8" s="77"/>
+      <c r="AQ8" s="88"/>
+      <c r="AR8" s="86"/>
       <c r="AS8" s="2" t="s">
         <v>31</v>
       </c>
@@ -2059,8 +2059,8 @@
       <c r="AU8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AV8" s="75"/>
-      <c r="AW8" s="77"/>
+      <c r="AV8" s="88"/>
+      <c r="AW8" s="86"/>
       <c r="AX8" s="2" t="s">
         <v>31</v>
       </c>
@@ -2070,11 +2070,11 @@
       <c r="AZ8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="BA8" s="75"/>
-      <c r="BB8" s="77"/>
-      <c r="BC8" s="75"/>
-      <c r="BD8" s="75"/>
-      <c r="BE8" s="77"/>
+      <c r="BA8" s="88"/>
+      <c r="BB8" s="86"/>
+      <c r="BC8" s="88"/>
+      <c r="BD8" s="88"/>
+      <c r="BE8" s="86"/>
       <c r="BF8" s="2" t="s">
         <v>31</v>
       </c>
@@ -2084,8 +2084,8 @@
       <c r="BH8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="BI8" s="75"/>
-      <c r="BJ8" s="77"/>
+      <c r="BI8" s="88"/>
+      <c r="BJ8" s="86"/>
       <c r="BK8" s="2" t="s">
         <v>31</v>
       </c>
@@ -2095,8 +2095,8 @@
       <c r="BM8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="BN8" s="75"/>
-      <c r="BO8" s="77"/>
+      <c r="BN8" s="88"/>
+      <c r="BO8" s="86"/>
       <c r="BP8" s="2" t="s">
         <v>31</v>
       </c>
@@ -2106,11 +2106,11 @@
       <c r="BR8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="BS8" s="75"/>
-      <c r="BT8" s="77"/>
-      <c r="BU8" s="75"/>
-      <c r="BV8" s="75"/>
-      <c r="BW8" s="75"/>
+      <c r="BS8" s="88"/>
+      <c r="BT8" s="86"/>
+      <c r="BU8" s="88"/>
+      <c r="BV8" s="88"/>
+      <c r="BW8" s="88"/>
       <c r="BX8" s="2" t="s">
         <v>31</v>
       </c>
@@ -2120,9 +2120,9 @@
       <c r="BZ8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="CA8" s="75"/>
-      <c r="CB8" s="72"/>
-      <c r="CC8" s="72"/>
+      <c r="CA8" s="88"/>
+      <c r="CB8" s="95"/>
+      <c r="CC8" s="95"/>
       <c r="CD8" s="3"/>
     </row>
     <row r="9" spans="1:82" s="14" customFormat="1" ht="15" customHeight="1">
@@ -2130,7 +2130,7 @@
         <v>34</v>
       </c>
       <c r="B9" s="15"/>
-      <c r="C9" s="94"/>
+      <c r="C9" s="67"/>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
@@ -2213,7 +2213,7 @@
     <row r="10" spans="1:82" s="14" customFormat="1" ht="15" customHeight="1">
       <c r="A10" s="41"/>
       <c r="B10" s="15"/>
-      <c r="C10" s="94"/>
+      <c r="C10" s="67"/>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
@@ -2296,7 +2296,7 @@
     <row r="11" spans="1:82" s="14" customFormat="1" ht="15" customHeight="1">
       <c r="A11" s="41"/>
       <c r="B11" s="15"/>
-      <c r="C11" s="94"/>
+      <c r="C11" s="67"/>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
@@ -2379,7 +2379,7 @@
     <row r="12" spans="1:82" s="14" customFormat="1" ht="15" customHeight="1">
       <c r="A12" s="41"/>
       <c r="B12" s="15"/>
-      <c r="C12" s="94"/>
+      <c r="C12" s="67"/>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
@@ -2462,7 +2462,7 @@
     <row r="13" spans="1:82" s="13" customFormat="1" ht="15.6">
       <c r="A13" s="41"/>
       <c r="B13" s="15"/>
-      <c r="C13" s="94"/>
+      <c r="C13" s="67"/>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
@@ -2545,7 +2545,7 @@
     <row r="14" spans="1:82" s="13" customFormat="1" ht="15.6">
       <c r="A14" s="41"/>
       <c r="B14" s="15"/>
-      <c r="C14" s="94"/>
+      <c r="C14" s="67"/>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
@@ -2628,7 +2628,7 @@
     <row r="15" spans="1:82" s="13" customFormat="1" ht="15.6">
       <c r="A15" s="41"/>
       <c r="B15" s="15"/>
-      <c r="C15" s="94"/>
+      <c r="C15" s="67"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
@@ -2711,7 +2711,7 @@
     <row r="16" spans="1:82" s="13" customFormat="1" ht="15.6">
       <c r="A16" s="41"/>
       <c r="B16" s="15"/>
-      <c r="C16" s="94"/>
+      <c r="C16" s="67"/>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
@@ -2794,7 +2794,7 @@
     <row r="17" spans="1:81" s="13" customFormat="1" ht="15.6">
       <c r="A17" s="41"/>
       <c r="B17" s="15"/>
-      <c r="C17" s="94"/>
+      <c r="C17" s="67"/>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
@@ -2877,7 +2877,7 @@
     <row r="18" spans="1:81" s="13" customFormat="1" ht="15.6">
       <c r="A18" s="41"/>
       <c r="B18" s="15"/>
-      <c r="C18" s="94"/>
+      <c r="C18" s="67"/>
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
       <c r="F18" s="24"/>
@@ -2960,7 +2960,7 @@
     <row r="19" spans="1:81" ht="15.6">
       <c r="A19" s="42"/>
       <c r="B19" s="26"/>
-      <c r="C19" s="95"/>
+      <c r="C19" s="68"/>
       <c r="D19" s="27"/>
       <c r="E19" s="27"/>
       <c r="F19" s="27"/>
@@ -3043,7 +3043,7 @@
     <row r="20" spans="1:81" ht="15.6">
       <c r="A20" s="42"/>
       <c r="B20" s="26"/>
-      <c r="C20" s="95"/>
+      <c r="C20" s="68"/>
       <c r="D20" s="27"/>
       <c r="E20" s="27"/>
       <c r="F20" s="27"/>
@@ -3126,7 +3126,7 @@
     <row r="21" spans="1:81" ht="15.6">
       <c r="A21" s="42"/>
       <c r="B21" s="26"/>
-      <c r="C21" s="95"/>
+      <c r="C21" s="68"/>
       <c r="D21" s="30"/>
       <c r="E21" s="30"/>
       <c r="F21" s="30"/>
@@ -3209,7 +3209,7 @@
     <row r="22" spans="1:81" ht="15.6">
       <c r="A22" s="42"/>
       <c r="B22" s="26"/>
-      <c r="C22" s="95"/>
+      <c r="C22" s="68"/>
       <c r="D22" s="31"/>
       <c r="E22" s="31"/>
       <c r="F22" s="31"/>
@@ -3292,7 +3292,7 @@
     <row r="23" spans="1:81" ht="15.6">
       <c r="A23" s="42"/>
       <c r="B23" s="26"/>
-      <c r="C23" s="95"/>
+      <c r="C23" s="68"/>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
       <c r="F23" s="27"/>
@@ -3375,7 +3375,7 @@
     <row r="24" spans="1:81" ht="15.6">
       <c r="A24" s="42"/>
       <c r="B24" s="26"/>
-      <c r="C24" s="95"/>
+      <c r="C24" s="68"/>
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
       <c r="F24" s="27"/>
@@ -3458,7 +3458,7 @@
     <row r="25" spans="1:81" ht="15.6">
       <c r="A25" s="42"/>
       <c r="B25" s="26"/>
-      <c r="C25" s="95"/>
+      <c r="C25" s="68"/>
       <c r="D25" s="32"/>
       <c r="E25" s="32"/>
       <c r="F25" s="32"/>
@@ -3541,7 +3541,7 @@
     <row r="26" spans="1:81" ht="15.6">
       <c r="A26" s="42"/>
       <c r="B26" s="26"/>
-      <c r="C26" s="95"/>
+      <c r="C26" s="68"/>
       <c r="D26" s="27"/>
       <c r="E26" s="27"/>
       <c r="F26" s="27"/>
@@ -3624,7 +3624,7 @@
     <row r="27" spans="1:81" ht="15.6">
       <c r="A27" s="42"/>
       <c r="B27" s="26"/>
-      <c r="C27" s="95"/>
+      <c r="C27" s="68"/>
       <c r="D27" s="27"/>
       <c r="E27" s="27"/>
       <c r="F27" s="27"/>
@@ -3707,7 +3707,7 @@
     <row r="28" spans="1:81" ht="15.6">
       <c r="A28" s="42"/>
       <c r="B28" s="26"/>
-      <c r="C28" s="95"/>
+      <c r="C28" s="68"/>
       <c r="D28" s="34"/>
       <c r="E28" s="34"/>
       <c r="F28" s="34"/>
@@ -3790,7 +3790,7 @@
     <row r="29" spans="1:81" ht="15.6">
       <c r="A29" s="42"/>
       <c r="B29" s="26"/>
-      <c r="C29" s="95"/>
+      <c r="C29" s="68"/>
       <c r="D29" s="35"/>
       <c r="E29" s="35"/>
       <c r="F29" s="35"/>
@@ -3873,7 +3873,7 @@
     <row r="30" spans="1:81" ht="15.6">
       <c r="A30" s="42"/>
       <c r="B30" s="26"/>
-      <c r="C30" s="95"/>
+      <c r="C30" s="68"/>
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
       <c r="F30" s="27"/>
@@ -3956,7 +3956,7 @@
     <row r="31" spans="1:81" ht="15.6">
       <c r="A31" s="42"/>
       <c r="B31" s="26"/>
-      <c r="C31" s="95"/>
+      <c r="C31" s="68"/>
       <c r="D31" s="36"/>
       <c r="E31" s="36"/>
       <c r="F31" s="36"/>
@@ -4039,7 +4039,7 @@
     <row r="32" spans="1:81" ht="15.6">
       <c r="A32" s="42"/>
       <c r="B32" s="26"/>
-      <c r="C32" s="95"/>
+      <c r="C32" s="68"/>
       <c r="D32" s="38"/>
       <c r="E32" s="38"/>
       <c r="F32" s="38"/>
@@ -4122,7 +4122,7 @@
     <row r="33" spans="1:81" ht="15.6">
       <c r="A33" s="42"/>
       <c r="B33" s="26"/>
-      <c r="C33" s="95"/>
+      <c r="C33" s="68"/>
       <c r="D33" s="40"/>
       <c r="E33" s="40"/>
       <c r="F33" s="40"/>
@@ -4207,7 +4207,7 @@
       <c r="B34" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="96">
+      <c r="C34" s="69">
         <f>SUM(C9:C33)</f>
         <v>0</v>
       </c>
@@ -4535,13 +4535,62 @@
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="BX4:CA6"/>
-    <mergeCell ref="D4:BE4"/>
-    <mergeCell ref="D5:R5"/>
-    <mergeCell ref="S5:U6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="I6:M6"/>
-    <mergeCell ref="N6:R6"/>
+    <mergeCell ref="BP7:BR7"/>
+    <mergeCell ref="CC4:CC8"/>
+    <mergeCell ref="A1:CC1"/>
+    <mergeCell ref="A2:CC2"/>
+    <mergeCell ref="BV7:BV8"/>
+    <mergeCell ref="BW7:BW8"/>
+    <mergeCell ref="CA7:CA8"/>
+    <mergeCell ref="CB4:CB8"/>
+    <mergeCell ref="BE7:BE8"/>
+    <mergeCell ref="BF5:BT5"/>
+    <mergeCell ref="BU5:BW6"/>
+    <mergeCell ref="BF6:BJ6"/>
+    <mergeCell ref="BK6:BO6"/>
+    <mergeCell ref="BP6:BT6"/>
+    <mergeCell ref="BF7:BH7"/>
+    <mergeCell ref="BI7:BI8"/>
+    <mergeCell ref="AN7:AP7"/>
+    <mergeCell ref="BJ7:BJ8"/>
+    <mergeCell ref="BK7:BM7"/>
+    <mergeCell ref="BN7:BN8"/>
+    <mergeCell ref="BO7:BO8"/>
+    <mergeCell ref="AD7:AD8"/>
+    <mergeCell ref="BC5:BE6"/>
+    <mergeCell ref="AN6:AR6"/>
+    <mergeCell ref="AS6:AW6"/>
+    <mergeCell ref="AX6:BB6"/>
+    <mergeCell ref="AA6:AE6"/>
+    <mergeCell ref="AF6:AJ6"/>
+    <mergeCell ref="V5:AJ5"/>
+    <mergeCell ref="V6:Z6"/>
+    <mergeCell ref="AK5:AM6"/>
+    <mergeCell ref="AQ7:AQ8"/>
+    <mergeCell ref="AR7:AR8"/>
+    <mergeCell ref="AS7:AU7"/>
+    <mergeCell ref="AV7:AV8"/>
+    <mergeCell ref="AN5:BB5"/>
+    <mergeCell ref="BC7:BC8"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="V7:X7"/>
+    <mergeCell ref="Y7:Y8"/>
+    <mergeCell ref="Z7:Z8"/>
+    <mergeCell ref="AA7:AC7"/>
+    <mergeCell ref="S7:S8"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="C4:C8"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="G7:G8"/>
     <mergeCell ref="BX7:BZ7"/>
     <mergeCell ref="AE7:AE8"/>
     <mergeCell ref="AF7:AH7"/>
@@ -4558,62 +4607,13 @@
     <mergeCell ref="AK7:AK8"/>
     <mergeCell ref="AL7:AL8"/>
     <mergeCell ref="AM7:AM8"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="C4:C8"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="R7:R8"/>
-    <mergeCell ref="V7:X7"/>
-    <mergeCell ref="Y7:Y8"/>
-    <mergeCell ref="Z7:Z8"/>
-    <mergeCell ref="AA7:AC7"/>
-    <mergeCell ref="S7:S8"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="AD7:AD8"/>
-    <mergeCell ref="BC5:BE6"/>
-    <mergeCell ref="AN6:AR6"/>
-    <mergeCell ref="AS6:AW6"/>
-    <mergeCell ref="AX6:BB6"/>
-    <mergeCell ref="AA6:AE6"/>
-    <mergeCell ref="AF6:AJ6"/>
-    <mergeCell ref="V5:AJ5"/>
-    <mergeCell ref="V6:Z6"/>
-    <mergeCell ref="AK5:AM6"/>
-    <mergeCell ref="AQ7:AQ8"/>
-    <mergeCell ref="AR7:AR8"/>
-    <mergeCell ref="AS7:AU7"/>
-    <mergeCell ref="AV7:AV8"/>
-    <mergeCell ref="AN5:BB5"/>
-    <mergeCell ref="BC7:BC8"/>
-    <mergeCell ref="AN7:AP7"/>
-    <mergeCell ref="BJ7:BJ8"/>
-    <mergeCell ref="BK7:BM7"/>
-    <mergeCell ref="BN7:BN8"/>
-    <mergeCell ref="BO7:BO8"/>
-    <mergeCell ref="BP7:BR7"/>
-    <mergeCell ref="CC4:CC8"/>
-    <mergeCell ref="A1:CC1"/>
-    <mergeCell ref="A2:CC2"/>
-    <mergeCell ref="BV7:BV8"/>
-    <mergeCell ref="BW7:BW8"/>
-    <mergeCell ref="CA7:CA8"/>
-    <mergeCell ref="CB4:CB8"/>
-    <mergeCell ref="BE7:BE8"/>
-    <mergeCell ref="BF5:BT5"/>
-    <mergeCell ref="BU5:BW6"/>
-    <mergeCell ref="BF6:BJ6"/>
-    <mergeCell ref="BK6:BO6"/>
-    <mergeCell ref="BP6:BT6"/>
-    <mergeCell ref="BF7:BH7"/>
-    <mergeCell ref="BI7:BI8"/>
+    <mergeCell ref="BX4:CA6"/>
+    <mergeCell ref="D4:BE4"/>
+    <mergeCell ref="D5:R5"/>
+    <mergeCell ref="S5:U6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="I6:M6"/>
+    <mergeCell ref="N6:R6"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="256" scale="70" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>